<commit_message>
EPBDS special test-end marker used - <END-OF-FUNCTIONS>
</commit_message>
<xml_diff>
--- a/POI/trunk/org.openl.lib.poi35.dev.modified/test-data/spreadsheet/ArrayFormulaFunctions.xlsx
+++ b/POI/trunk/org.openl.lib.poi35.dev.modified/test-data/spreadsheet/ArrayFormulaFunctions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="315" windowWidth="18720" windowHeight="11640"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Array Formula  Functions Test</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Simple tests</t>
   </si>
   <si>
-    <t>END</t>
-  </si>
-  <si>
     <t>horizontal array</t>
   </si>
   <si>
@@ -109,13 +106,22 @@
   </si>
   <si>
     <t>ref array in array</t>
+  </si>
+  <si>
+    <t>&lt;END-OF-FUNCTIONS&gt;</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Expected value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,13 +129,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,17 +175,92 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -163,7 +272,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="D4D0C8"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -442,18 +551,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -462,14 +578,14 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="C4">
+      <c r="C4" s="2">
         <f t="array" ref="C4:E4">SQRT({1,4,16})</f>
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
         <v>4</v>
       </c>
       <c r="I4">
@@ -482,18 +598,18 @@
         <v>4</v>
       </c>
       <c r="N4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="C6">
+      <c r="C6" s="3">
         <f t="array" ref="C6:E7">SQRT({1,4,16;9,25,36})</f>
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
         <v>4</v>
       </c>
       <c r="I6">
@@ -506,17 +622,17 @@
         <v>4</v>
       </c>
       <c r="N6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
         <v>5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>6</v>
       </c>
       <c r="I7">
@@ -530,7 +646,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="C9">
+      <c r="C9" s="2">
         <f t="array" ref="C9:C11">SQRT({9;25;36})</f>
         <v>3</v>
       </c>
@@ -538,11 +654,11 @@
         <v>3</v>
       </c>
       <c r="N9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="C10">
+      <c r="C10" s="2">
         <v>5</v>
       </c>
       <c r="I10">
@@ -550,7 +666,7 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="C11">
+      <c r="C11" s="2">
         <v>6</v>
       </c>
       <c r="I11">
@@ -574,11 +690,11 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="C16">
+      <c r="C16" s="3">
         <f t="array" ref="C16:D16">POWER(A14:B14,A15:B15)</f>
         <v>2</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>9</v>
       </c>
       <c r="I16">
@@ -588,12 +704,12 @@
         <v>9</v>
       </c>
       <c r="N16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="G19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -621,7 +737,7 @@
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="C23">
+      <c r="C23" s="2">
         <f t="array" ref="C23:C25">INDEX(A20:B22,0,2)</f>
         <v>2</v>
       </c>
@@ -629,11 +745,11 @@
         <v>2</v>
       </c>
       <c r="N23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="C24">
+      <c r="C24" s="2">
         <v>4</v>
       </c>
       <c r="I24">
@@ -641,7 +757,7 @@
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="C25">
+      <c r="C25" s="2">
         <v>6</v>
       </c>
       <c r="I25">
@@ -681,11 +797,11 @@
       </c>
     </row>
     <row r="33" spans="1:14">
-      <c r="C33">
+      <c r="C33" s="3">
         <f t="array" ref="C33:D34">A28:B29*A31:B32</f>
         <v>5</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="3">
         <v>12</v>
       </c>
       <c r="I33">
@@ -695,14 +811,14 @@
         <v>12</v>
       </c>
       <c r="N33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:14">
-      <c r="C34">
+      <c r="C34" s="3">
         <v>21</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="3">
         <v>32</v>
       </c>
       <c r="I34">
@@ -714,7 +830,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="G37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -734,7 +850,7 @@
       </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="C41">
+      <c r="C41" s="2">
         <f t="array" ref="C41">SUM(A39:A40*B39:B40)</f>
         <v>14</v>
       </c>
@@ -742,7 +858,7 @@
         <v>14</v>
       </c>
       <c r="N41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -763,7 +879,7 @@
       </c>
     </row>
     <row r="48" spans="1:14">
-      <c r="C48">
+      <c r="C48" s="3">
         <f t="array" ref="C48">SUM(A45:E45*{1,2,3,4,5})</f>
         <v>55</v>
       </c>
@@ -771,11 +887,11 @@
         <v>55</v>
       </c>
       <c r="N48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="C50">
+      <c r="C50" s="2">
         <f t="array" ref="C50">SUM({1,2,3,4,5}*{1,2,3,4,5})</f>
         <v>55</v>
       </c>
@@ -783,21 +899,21 @@
         <v>55</v>
       </c>
       <c r="N50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:14">
-      <c r="C55">
+      <c r="C55" s="2">
         <f t="array" ref="C55:F57">{1,2,3,4;5,6,7,8;9,10,11,12}*2</f>
         <v>2</v>
       </c>
-      <c r="D55">
-        <v>4</v>
-      </c>
-      <c r="E55">
+      <c r="D55" s="2">
+        <v>4</v>
+      </c>
+      <c r="E55" s="2">
         <v>6</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="2">
         <v>8</v>
       </c>
       <c r="I55">
@@ -813,20 +929,20 @@
         <v>8</v>
       </c>
       <c r="N55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="C56">
+      <c r="C56" s="2">
         <v>10</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="2">
         <v>12</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="2">
         <v>14</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="2">
         <v>16</v>
       </c>
       <c r="I56">
@@ -843,16 +959,16 @@
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="C57">
+      <c r="C57" s="2">
         <v>18</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="2">
         <v>20</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="2">
         <v>22</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="2">
         <v>24</v>
       </c>
       <c r="I57">
@@ -870,22 +986,22 @@
     </row>
     <row r="61" spans="1:14">
       <c r="A61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" t="s">
         <v>14</v>
-      </c>
-      <c r="B61" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:14">
       <c r="A62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" t="s">
         <v>16</v>
       </c>
-      <c r="B62" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="C63">
+      <c r="C63" s="3">
         <f t="array" ref="C63">SUM(LEN(A61:B62))</f>
         <v>13</v>
       </c>
@@ -893,7 +1009,7 @@
         <v>13</v>
       </c>
       <c r="N63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -913,11 +1029,11 @@
       </c>
     </row>
     <row r="69" spans="1:14">
-      <c r="C69">
+      <c r="C69" s="2">
         <f t="array" ref="C69:D69">SMALL(A67:B68,{1,2})</f>
         <v>1</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="2">
         <v>2</v>
       </c>
       <c r="I69">
@@ -927,23 +1043,23 @@
         <v>2</v>
       </c>
       <c r="N69" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="C72" s="3">
+        <f>AVERAGE(SMALL(A67:B68,{2,4}))</f>
+        <v>3</v>
+      </c>
+      <c r="I72">
+        <v>3</v>
+      </c>
+      <c r="N72" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
-      <c r="C72">
-        <f>AVERAGE(SMALL(A67:B68,{2,4}))</f>
-        <v>3</v>
-      </c>
-      <c r="I72">
-        <v>3</v>
-      </c>
-      <c r="N72" t="s">
-        <v>21</v>
-      </c>
-    </row>
     <row r="75" spans="1:14">
-      <c r="C75">
+      <c r="C75" s="2">
         <f t="array" ref="C75">SUM(IF(A67:B68&gt;2,A67:B68,1))</f>
         <v>9</v>
       </c>
@@ -951,11 +1067,11 @@
         <v>9</v>
       </c>
       <c r="N75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:14">
-      <c r="C78">
+      <c r="C78" s="3">
         <f t="array" ref="C78">SUM(IF((A67:B68&gt;3)+(A67:B68&lt;2),A67:B68))</f>
         <v>5</v>
       </c>
@@ -963,7 +1079,7 @@
         <v>5</v>
       </c>
       <c r="N78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:14">
@@ -991,7 +1107,7 @@
       </c>
     </row>
     <row r="84" spans="1:14">
-      <c r="C84">
+      <c r="C84" s="2">
         <f t="array" ref="C84">SUM(IF(A81:A83=B81:B83,0,1))</f>
         <v>2</v>
       </c>
@@ -999,21 +1115,21 @@
         <v>2</v>
       </c>
       <c r="N84" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:14">
-      <c r="C87">
+      <c r="C87" s="3">
         <f t="array" ref="C87:F87">COLUMN(A1:E10)</f>
         <v>1</v>
       </c>
-      <c r="D87">
-        <v>2</v>
-      </c>
-      <c r="E87">
-        <v>3</v>
-      </c>
-      <c r="F87">
+      <c r="D87" s="3">
+        <v>2</v>
+      </c>
+      <c r="E87" s="3">
+        <v>3</v>
+      </c>
+      <c r="F87" s="3">
         <v>4</v>
       </c>
       <c r="I87">
@@ -1029,23 +1145,23 @@
         <v>4</v>
       </c>
       <c r="N87" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14">
+      <c r="C88" s="2">
+        <f>SUM(COLUMN(A1:E10))</f>
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="N88" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
-      <c r="C88">
-        <f>SUM(COLUMN(A1:E10))</f>
-        <v>1</v>
-      </c>
-      <c r="I88">
-        <v>1</v>
-      </c>
-      <c r="N88" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="89" spans="1:14">
-      <c r="C89">
+      <c r="C89" s="3">
         <f t="array" ref="C89">SUM(COLUMN(A1:E10))</f>
         <v>15</v>
       </c>
@@ -1053,11 +1169,11 @@
         <v>15</v>
       </c>
       <c r="N89" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="1:14">
-      <c r="C90">
+      <c r="C90" s="2">
         <f t="array" ref="C90:C94">ROW(A1:A10)</f>
         <v>1</v>
       </c>
@@ -1065,11 +1181,11 @@
         <v>1</v>
       </c>
       <c r="N90" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:14">
-      <c r="C91">
+      <c r="C91" s="2">
         <v>2</v>
       </c>
       <c r="I91">
@@ -1077,7 +1193,7 @@
       </c>
     </row>
     <row r="92" spans="1:14">
-      <c r="C92">
+      <c r="C92" s="2">
         <v>3</v>
       </c>
       <c r="I92">
@@ -1085,7 +1201,7 @@
       </c>
     </row>
     <row r="93" spans="1:14">
-      <c r="C93">
+      <c r="C93" s="2">
         <v>4</v>
       </c>
       <c r="I93">
@@ -1093,7 +1209,7 @@
       </c>
     </row>
     <row r="94" spans="1:14">
-      <c r="C94">
+      <c r="C94" s="2">
         <v>5</v>
       </c>
       <c r="I94">
@@ -1118,7 +1234,7 @@
       </c>
     </row>
     <row r="99" spans="1:14">
-      <c r="C99">
+      <c r="C99" s="3">
         <f>B98+1</f>
         <v>3</v>
       </c>
@@ -1126,15 +1242,15 @@
         <v>3</v>
       </c>
       <c r="N99" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="102" spans="1:14">
-      <c r="B102">
+      <c r="B102" s="2">
         <f t="array" ref="B102:C103">A97:B98+1</f>
         <v>2</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="2">
         <v>2.4142135623730949</v>
       </c>
       <c r="I102">
@@ -1144,14 +1260,14 @@
         <v>2.4142135623730949</v>
       </c>
       <c r="N102" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="103" spans="1:14">
-      <c r="B103">
+      <c r="B103" s="2">
         <v>2.7320508075688772</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="2">
         <v>3</v>
       </c>
       <c r="I103">
@@ -1162,15 +1278,13 @@
       </c>
     </row>
     <row r="110" spans="1:14">
-      <c r="H110" t="s">
-        <v>2</v>
-      </c>
-      <c r="I110" t="s">
-        <v>2</v>
+      <c r="C110" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>